<commit_message>
check-point 19 July 2023
</commit_message>
<xml_diff>
--- a/Python/PercobaanVoiceRecognition/asset/sound/Sample that needs to made.xlsx
+++ b/Python/PercobaanVoiceRecognition/asset/sound/Sample that needs to made.xlsx
@@ -616,11 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:E85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -637,7 +636,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -733,7 +732,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -877,7 +876,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="22" spans="1:5" hidden="1">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>66</v>
       </c>
@@ -925,7 +924,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="26" spans="1:5" hidden="1">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>82</v>
       </c>
@@ -937,7 +936,7 @@
         <v>B</v>
       </c>
     </row>
-    <row r="27" spans="1:5" hidden="1">
+    <row r="27" spans="1:5">
       <c r="D27" s="1" t="s">
         <v>25</v>
       </c>
@@ -946,7 +945,7 @@
         <v>CH</v>
       </c>
     </row>
-    <row r="28" spans="1:5" hidden="1">
+    <row r="28" spans="1:5">
       <c r="D28" s="1" t="s">
         <v>26</v>
       </c>
@@ -964,7 +963,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="30" spans="1:5" hidden="1">
+    <row r="30" spans="1:5">
       <c r="D30" s="1" t="s">
         <v>28</v>
       </c>
@@ -1036,7 +1035,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="38" spans="4:5" hidden="1">
+    <row r="38" spans="4:5">
       <c r="D38" s="1" t="s">
         <v>36</v>
       </c>
@@ -1072,7 +1071,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="42" spans="4:5" hidden="1">
+    <row r="42" spans="4:5">
       <c r="D42" s="1" t="s">
         <v>40</v>
       </c>
@@ -1135,7 +1134,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="49" spans="4:5" hidden="1">
+    <row r="49" spans="4:5">
       <c r="D49" s="1" t="s">
         <v>47</v>
       </c>
@@ -1171,7 +1170,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="53" spans="4:5" hidden="1">
+    <row r="53" spans="4:5">
       <c r="D53" s="1" t="s">
         <v>51</v>
       </c>
@@ -1180,7 +1179,7 @@
         <v>JH</v>
       </c>
     </row>
-    <row r="54" spans="4:5" hidden="1">
+    <row r="54" spans="4:5">
       <c r="D54" s="1" t="s">
         <v>52</v>
       </c>
@@ -1189,7 +1188,7 @@
         <v>K</v>
       </c>
     </row>
-    <row r="55" spans="4:5" hidden="1">
+    <row r="55" spans="4:5">
       <c r="D55" s="1" t="s">
         <v>53</v>
       </c>
@@ -1198,7 +1197,7 @@
         <v>L</v>
       </c>
     </row>
-    <row r="56" spans="4:5" hidden="1">
+    <row r="56" spans="4:5">
       <c r="D56" s="1" t="s">
         <v>54</v>
       </c>
@@ -1207,7 +1206,7 @@
         <v>M</v>
       </c>
     </row>
-    <row r="57" spans="4:5" hidden="1">
+    <row r="57" spans="4:5">
       <c r="D57" s="1" t="s">
         <v>55</v>
       </c>
@@ -1225,7 +1224,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="59" spans="4:5" hidden="1">
+    <row r="59" spans="4:5">
       <c r="D59" s="1" t="s">
         <v>57</v>
       </c>
@@ -1297,7 +1296,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="67" spans="4:5" hidden="1">
+    <row r="67" spans="4:5">
       <c r="D67" s="1" t="s">
         <v>65</v>
       </c>
@@ -1306,7 +1305,7 @@
         <v>P</v>
       </c>
     </row>
-    <row r="68" spans="4:5" hidden="1">
+    <row r="68" spans="4:5">
       <c r="D68" s="1" t="s">
         <v>66</v>
       </c>
@@ -1315,7 +1314,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="69" spans="4:5" hidden="1">
+    <row r="69" spans="4:5">
       <c r="D69" s="1" t="s">
         <v>67</v>
       </c>
@@ -1333,7 +1332,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="71" spans="4:5" hidden="1">
+    <row r="71" spans="4:5">
       <c r="D71" s="1" t="s">
         <v>69</v>
       </c>
@@ -1387,7 +1386,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="77" spans="4:5" hidden="1">
+    <row r="77" spans="4:5">
       <c r="D77" s="1" t="s">
         <v>75</v>
       </c>
@@ -1423,7 +1422,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="81" spans="4:5" hidden="1">
+    <row r="81" spans="4:5">
       <c r="D81" s="1" t="s">
         <v>79</v>
       </c>
@@ -1432,7 +1431,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="82" spans="4:5" hidden="1">
+    <row r="82" spans="4:5">
       <c r="D82" s="1" t="s">
         <v>80</v>
       </c>
@@ -1441,7 +1440,7 @@
         <v>W</v>
       </c>
     </row>
-    <row r="83" spans="4:5" hidden="1">
+    <row r="83" spans="4:5">
       <c r="D83" s="1" t="s">
         <v>81</v>
       </c>
@@ -1450,7 +1449,7 @@
         <v>Y</v>
       </c>
     </row>
-    <row r="84" spans="4:5" hidden="1">
+    <row r="84" spans="4:5">
       <c r="D84" s="1" t="s">
         <v>82</v>
       </c>
@@ -1469,13 +1468,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="D1:E85">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="#N/A"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="D1:E85"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>